<commit_message>
Update the data of material properties
For the better prediction, remove the outlier of
material properties.
</commit_message>
<xml_diff>
--- a/data/glcm-data/第一批狗骨頭材料特性.xlsx
+++ b/data/glcm-data/第一批狗骨頭材料特性.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>trail</t>
   </si>
@@ -82,7 +82,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -91,6 +91,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
@@ -375,11 +378,11 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="1">
-        <v>318.9186</v>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
       </c>
-      <c r="G2" s="1">
-        <v>304.4544</v>
+      <c r="G2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -439,7 +442,7 @@
       <c r="G4" s="1">
         <v>433.6858</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="4"/>
       <c r="Q4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
@@ -468,7 +471,7 @@
       <c r="G5" s="1">
         <v>189.419</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
@@ -497,7 +500,7 @@
       <c r="G6" s="1">
         <v>274.9841</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="4"/>
       <c r="Q6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
@@ -514,8 +517,8 @@
       <c r="C7" s="1">
         <v>383.4766</v>
       </c>
-      <c r="D7" s="1">
-        <v>362.5309</v>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E7" s="1">
         <v>403.5413</v>
@@ -526,7 +529,7 @@
       <c r="G7" s="1">
         <v>396.1015</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
@@ -555,7 +558,7 @@
       <c r="G8" s="1">
         <v>160.5596</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="4"/>
       <c r="Q8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
@@ -584,7 +587,7 @@
       <c r="G9" s="1">
         <v>266.8105</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
@@ -598,8 +601,8 @@
       <c r="B10" s="1">
         <v>361.7663</v>
       </c>
-      <c r="C10" s="1">
-        <v>315.9442</v>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1">
         <v>368.0783</v>
@@ -613,7 +616,7 @@
       <c r="G10" s="1">
         <v>378.635</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="P10" s="4"/>
       <c r="Q10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -621,7 +624,7 @@
       <c r="AJ10" s="2"/>
     </row>
     <row r="11">
-      <c r="P11" s="3"/>
+      <c r="P11" s="4"/>
       <c r="Q11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
@@ -642,9 +645,9 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>

</xml_diff>

<commit_message>
Update material property data
</commit_message>
<xml_diff>
--- a/data/glcm-data/第一批狗骨頭材料特性.xlsx
+++ b/data/glcm-data/第一批狗骨頭材料特性.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>oxygen concentration</t>
   </si>
@@ -63,7 +63,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +81,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -111,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -131,6 +137,9 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -140,14 +149,17 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -157,6 +169,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,42 +481,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="14" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="15" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="15" width="4.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="15" width="6.005" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="15" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="15" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="15" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="15" width="5.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="15" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="16" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="16" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="16" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="17" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="17" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="17" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="18" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="18" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="18" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="18" width="4.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="18" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="18" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="18" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="18" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="18" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="18" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="18" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="18" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="18" width="5.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="18" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="18" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="18" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="18" width="5.433571428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -546,40 +561,40 @@
       <c r="O1" s="5"/>
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AD1" s="5"/>
-      <c r="AE1" s="5"/>
-      <c r="AF1" s="5"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
       <c r="AG1" s="6"/>
       <c r="AH1" s="6"/>
       <c r="AI1" s="6"/>
       <c r="AJ1" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="7">
+      <c r="A2" s="8">
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="8">
         <v>150</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="8">
         <v>400</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="9">
         <v>0.05</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="9">
         <v>115.385</v>
       </c>
       <c r="F2" s="3">
@@ -597,51 +612,51 @@
       <c r="J2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>12</v>
+      <c r="K2" s="4">
+        <v>318.9186</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>12</v>
+      <c r="L2" s="4">
+        <v>304.4544</v>
       </c>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="7"/>
+      <c r="AD2" s="7"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
       <c r="AI2" s="6"/>
       <c r="AJ2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="7">
+      <c r="A3" s="8">
         <v>0</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="8">
         <v>200</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="8">
         <v>700</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>0.06</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>73.26</v>
       </c>
       <c r="F3" s="3">
@@ -670,40 +685,40 @@
       <c r="O3" s="5"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
       <c r="AI3" s="6"/>
       <c r="AJ3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="7">
+      <c r="A4" s="8">
         <v>0</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="8">
         <v>250</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="8">
         <v>1000</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>0.07</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>54.945</v>
       </c>
       <c r="F4" s="3">
@@ -730,42 +745,42 @@
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="9"/>
+      <c r="P4" s="10"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="5"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="5"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="5"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="5"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="5"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
       <c r="AI4" s="6"/>
       <c r="AJ4" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="7">
+      <c r="A5" s="8">
         <v>3000</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <v>150</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="8">
         <v>700</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="9">
         <v>0.07</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>47.096</v>
       </c>
       <c r="F5" s="3">
@@ -792,42 +807,42 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="9"/>
+      <c r="P5" s="10"/>
       <c r="Q5" s="6"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="5"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
       <c r="AJ5" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="7">
+      <c r="A6" s="8">
         <v>3000</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="8">
         <v>200</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="8">
         <v>1000</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>0.05</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="9">
         <v>61.538</v>
       </c>
       <c r="F6" s="3">
@@ -854,42 +869,42 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="9"/>
+      <c r="P6" s="10"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="5"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="7"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="6"/>
       <c r="AI6" s="6"/>
       <c r="AJ6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="7">
+      <c r="A7" s="8">
         <v>3000</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="8">
         <v>250</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="8">
         <v>400</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="9">
         <v>0.06</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="9">
         <v>160.256</v>
       </c>
       <c r="F7" s="3">
@@ -901,8 +916,8 @@
       <c r="H7" s="4">
         <v>383.4766</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>12</v>
+      <c r="I7" s="4">
+        <v>362.5309</v>
       </c>
       <c r="J7" s="4">
         <v>403.5413</v>
@@ -916,42 +931,42 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="9"/>
+      <c r="P7" s="10"/>
       <c r="Q7" s="6"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
-      <c r="W7" s="5"/>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
-      <c r="Z7" s="5"/>
-      <c r="AA7" s="5"/>
-      <c r="AB7" s="5"/>
-      <c r="AC7" s="5"/>
-      <c r="AD7" s="5"/>
-      <c r="AE7" s="5"/>
-      <c r="AF7" s="5"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="7"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="7"/>
       <c r="AG7" s="6"/>
       <c r="AH7" s="6"/>
       <c r="AI7" s="6"/>
       <c r="AJ7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="7">
+      <c r="A8" s="8">
         <v>6000</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="8">
         <v>150</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="8">
         <v>1000</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="9">
         <v>0.06</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>38.462</v>
       </c>
       <c r="F8" s="3">
@@ -978,42 +993,42 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
-      <c r="P8" s="9"/>
+      <c r="P8" s="10"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
       <c r="AJ8" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="7">
+      <c r="A9" s="8">
         <v>6000</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="8">
         <v>200</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="8">
         <v>400</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>0.07</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>109.89</v>
       </c>
       <c r="F9" s="3">
@@ -1040,42 +1055,42 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
-      <c r="P9" s="9"/>
+      <c r="P9" s="10"/>
       <c r="Q9" s="6"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
       <c r="AJ9" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="7">
+      <c r="A10" s="8">
         <v>6000</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="8">
         <v>250</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="8">
         <v>700</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <v>0.05</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>109.89</v>
       </c>
       <c r="F10" s="3">
@@ -1102,61 +1117,61 @@
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="9"/>
+      <c r="P10" s="10"/>
       <c r="Q10" s="6"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" s="5"/>
-      <c r="Z10" s="5"/>
-      <c r="AA10" s="5"/>
-      <c r="AB10" s="5"/>
-      <c r="AC10" s="5"/>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
       <c r="AG10" s="6"/>
       <c r="AH10" s="6"/>
       <c r="AI10" s="6"/>
       <c r="AJ10" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="9"/>
+      <c r="P11" s="10"/>
       <c r="Q11" s="6"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="5"/>
-      <c r="W11" s="5"/>
-      <c r="X11" s="5"/>
-      <c r="Y11" s="5"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="5"/>
-      <c r="AB11" s="5"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
       <c r="AG11" s="6"/>
       <c r="AH11" s="6"/>
       <c r="AI11" s="6"/>
@@ -1176,25 +1191,25 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
       <c r="Q12" s="6"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="5"/>
-      <c r="W12" s="5"/>
-      <c r="X12" s="5"/>
-      <c r="Y12" s="5"/>
-      <c r="Z12" s="5"/>
-      <c r="AA12" s="5"/>
-      <c r="AB12" s="5"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
       <c r="AG12" s="6"/>
       <c r="AH12" s="6"/>
       <c r="AI12" s="6"/>
@@ -36580,17 +36595,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="944" customHeight="1" ht="17.25">
       <c r="A944" s="1"/>
-      <c r="B944" s="10"/>
-      <c r="C944" s="10"/>
-      <c r="D944" s="11"/>
-      <c r="E944" s="11"/>
-      <c r="F944" s="10"/>
-      <c r="G944" s="11"/>
-      <c r="H944" s="11"/>
-      <c r="I944" s="11"/>
-      <c r="J944" s="11"/>
-      <c r="K944" s="11"/>
-      <c r="L944" s="11"/>
+      <c r="B944" s="11"/>
+      <c r="C944" s="11"/>
+      <c r="D944" s="12"/>
+      <c r="E944" s="12"/>
+      <c r="F944" s="11"/>
+      <c r="G944" s="12"/>
+      <c r="H944" s="12"/>
+      <c r="I944" s="12"/>
+      <c r="J944" s="12"/>
+      <c r="K944" s="12"/>
+      <c r="L944" s="12"/>
       <c r="M944" s="5"/>
       <c r="N944" s="5"/>
       <c r="O944" s="5"/>
@@ -36618,17 +36633,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="945" customHeight="1" ht="17.25">
       <c r="A945" s="1"/>
-      <c r="B945" s="10"/>
-      <c r="C945" s="10"/>
-      <c r="D945" s="11"/>
-      <c r="E945" s="11"/>
-      <c r="F945" s="10"/>
-      <c r="G945" s="11"/>
-      <c r="H945" s="11"/>
-      <c r="I945" s="11"/>
-      <c r="J945" s="11"/>
-      <c r="K945" s="11"/>
-      <c r="L945" s="11"/>
+      <c r="B945" s="11"/>
+      <c r="C945" s="11"/>
+      <c r="D945" s="12"/>
+      <c r="E945" s="12"/>
+      <c r="F945" s="11"/>
+      <c r="G945" s="12"/>
+      <c r="H945" s="12"/>
+      <c r="I945" s="12"/>
+      <c r="J945" s="12"/>
+      <c r="K945" s="12"/>
+      <c r="L945" s="12"/>
       <c r="M945" s="5"/>
       <c r="N945" s="5"/>
       <c r="O945" s="5"/>
@@ -36656,17 +36671,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="946" customHeight="1" ht="17.25">
       <c r="A946" s="1"/>
-      <c r="B946" s="10"/>
-      <c r="C946" s="10"/>
-      <c r="D946" s="11"/>
-      <c r="E946" s="11"/>
-      <c r="F946" s="10"/>
-      <c r="G946" s="11"/>
-      <c r="H946" s="11"/>
-      <c r="I946" s="11"/>
-      <c r="J946" s="11"/>
-      <c r="K946" s="11"/>
-      <c r="L946" s="11"/>
+      <c r="B946" s="11"/>
+      <c r="C946" s="11"/>
+      <c r="D946" s="12"/>
+      <c r="E946" s="12"/>
+      <c r="F946" s="11"/>
+      <c r="G946" s="12"/>
+      <c r="H946" s="12"/>
+      <c r="I946" s="12"/>
+      <c r="J946" s="12"/>
+      <c r="K946" s="12"/>
+      <c r="L946" s="12"/>
       <c r="M946" s="5"/>
       <c r="N946" s="5"/>
       <c r="O946" s="5"/>
@@ -36694,17 +36709,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="947" customHeight="1" ht="17.25">
       <c r="A947" s="1"/>
-      <c r="B947" s="10"/>
-      <c r="C947" s="10"/>
-      <c r="D947" s="11"/>
-      <c r="E947" s="11"/>
-      <c r="F947" s="10"/>
-      <c r="G947" s="11"/>
-      <c r="H947" s="11"/>
-      <c r="I947" s="11"/>
-      <c r="J947" s="11"/>
-      <c r="K947" s="11"/>
-      <c r="L947" s="11"/>
+      <c r="B947" s="11"/>
+      <c r="C947" s="11"/>
+      <c r="D947" s="12"/>
+      <c r="E947" s="12"/>
+      <c r="F947" s="11"/>
+      <c r="G947" s="12"/>
+      <c r="H947" s="12"/>
+      <c r="I947" s="12"/>
+      <c r="J947" s="12"/>
+      <c r="K947" s="12"/>
+      <c r="L947" s="12"/>
       <c r="M947" s="5"/>
       <c r="N947" s="5"/>
       <c r="O947" s="5"/>
@@ -36732,17 +36747,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="948" customHeight="1" ht="17.25">
       <c r="A948" s="1"/>
-      <c r="B948" s="10"/>
-      <c r="C948" s="10"/>
-      <c r="D948" s="11"/>
-      <c r="E948" s="11"/>
-      <c r="F948" s="10"/>
-      <c r="G948" s="11"/>
-      <c r="H948" s="11"/>
-      <c r="I948" s="11"/>
-      <c r="J948" s="11"/>
-      <c r="K948" s="11"/>
-      <c r="L948" s="11"/>
+      <c r="B948" s="11"/>
+      <c r="C948" s="11"/>
+      <c r="D948" s="12"/>
+      <c r="E948" s="12"/>
+      <c r="F948" s="11"/>
+      <c r="G948" s="12"/>
+      <c r="H948" s="12"/>
+      <c r="I948" s="12"/>
+      <c r="J948" s="12"/>
+      <c r="K948" s="12"/>
+      <c r="L948" s="12"/>
       <c r="M948" s="5"/>
       <c r="N948" s="5"/>
       <c r="O948" s="5"/>
@@ -36770,17 +36785,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="949" customHeight="1" ht="17.25">
       <c r="A949" s="1"/>
-      <c r="B949" s="10"/>
-      <c r="C949" s="10"/>
-      <c r="D949" s="11"/>
-      <c r="E949" s="11"/>
-      <c r="F949" s="10"/>
-      <c r="G949" s="11"/>
-      <c r="H949" s="11"/>
-      <c r="I949" s="11"/>
-      <c r="J949" s="11"/>
-      <c r="K949" s="11"/>
-      <c r="L949" s="11"/>
+      <c r="B949" s="11"/>
+      <c r="C949" s="11"/>
+      <c r="D949" s="12"/>
+      <c r="E949" s="12"/>
+      <c r="F949" s="11"/>
+      <c r="G949" s="12"/>
+      <c r="H949" s="12"/>
+      <c r="I949" s="12"/>
+      <c r="J949" s="12"/>
+      <c r="K949" s="12"/>
+      <c r="L949" s="12"/>
       <c r="M949" s="5"/>
       <c r="N949" s="5"/>
       <c r="O949" s="5"/>
@@ -36808,17 +36823,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="950" customHeight="1" ht="17.25">
       <c r="A950" s="1"/>
-      <c r="B950" s="10"/>
-      <c r="C950" s="10"/>
-      <c r="D950" s="11"/>
-      <c r="E950" s="11"/>
-      <c r="F950" s="10"/>
-      <c r="G950" s="11"/>
-      <c r="H950" s="11"/>
-      <c r="I950" s="11"/>
-      <c r="J950" s="11"/>
-      <c r="K950" s="11"/>
-      <c r="L950" s="11"/>
+      <c r="B950" s="11"/>
+      <c r="C950" s="11"/>
+      <c r="D950" s="12"/>
+      <c r="E950" s="12"/>
+      <c r="F950" s="11"/>
+      <c r="G950" s="12"/>
+      <c r="H950" s="12"/>
+      <c r="I950" s="12"/>
+      <c r="J950" s="12"/>
+      <c r="K950" s="12"/>
+      <c r="L950" s="12"/>
       <c r="M950" s="5"/>
       <c r="N950" s="5"/>
       <c r="O950" s="5"/>
@@ -36846,17 +36861,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="951" customHeight="1" ht="17.25">
       <c r="A951" s="1"/>
-      <c r="B951" s="10"/>
-      <c r="C951" s="10"/>
-      <c r="D951" s="11"/>
-      <c r="E951" s="11"/>
-      <c r="F951" s="10"/>
-      <c r="G951" s="11"/>
-      <c r="H951" s="11"/>
-      <c r="I951" s="11"/>
-      <c r="J951" s="11"/>
-      <c r="K951" s="11"/>
-      <c r="L951" s="11"/>
+      <c r="B951" s="11"/>
+      <c r="C951" s="11"/>
+      <c r="D951" s="12"/>
+      <c r="E951" s="12"/>
+      <c r="F951" s="11"/>
+      <c r="G951" s="12"/>
+      <c r="H951" s="12"/>
+      <c r="I951" s="12"/>
+      <c r="J951" s="12"/>
+      <c r="K951" s="12"/>
+      <c r="L951" s="12"/>
       <c r="M951" s="5"/>
       <c r="N951" s="5"/>
       <c r="O951" s="5"/>
@@ -36884,17 +36899,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="952" customHeight="1" ht="17.25">
       <c r="A952" s="1"/>
-      <c r="B952" s="10"/>
-      <c r="C952" s="10"/>
-      <c r="D952" s="11"/>
-      <c r="E952" s="11"/>
-      <c r="F952" s="10"/>
-      <c r="G952" s="11"/>
-      <c r="H952" s="11"/>
-      <c r="I952" s="11"/>
-      <c r="J952" s="11"/>
-      <c r="K952" s="11"/>
-      <c r="L952" s="11"/>
+      <c r="B952" s="11"/>
+      <c r="C952" s="11"/>
+      <c r="D952" s="12"/>
+      <c r="E952" s="12"/>
+      <c r="F952" s="11"/>
+      <c r="G952" s="12"/>
+      <c r="H952" s="12"/>
+      <c r="I952" s="12"/>
+      <c r="J952" s="12"/>
+      <c r="K952" s="12"/>
+      <c r="L952" s="12"/>
       <c r="M952" s="5"/>
       <c r="N952" s="5"/>
       <c r="O952" s="5"/>
@@ -36922,17 +36937,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="953" customHeight="1" ht="17.25">
       <c r="A953" s="1"/>
-      <c r="B953" s="10"/>
-      <c r="C953" s="10"/>
-      <c r="D953" s="11"/>
-      <c r="E953" s="11"/>
-      <c r="F953" s="10"/>
-      <c r="G953" s="11"/>
-      <c r="H953" s="11"/>
-      <c r="I953" s="11"/>
-      <c r="J953" s="11"/>
-      <c r="K953" s="11"/>
-      <c r="L953" s="11"/>
+      <c r="B953" s="11"/>
+      <c r="C953" s="11"/>
+      <c r="D953" s="12"/>
+      <c r="E953" s="12"/>
+      <c r="F953" s="11"/>
+      <c r="G953" s="12"/>
+      <c r="H953" s="12"/>
+      <c r="I953" s="12"/>
+      <c r="J953" s="12"/>
+      <c r="K953" s="12"/>
+      <c r="L953" s="12"/>
       <c r="M953" s="5"/>
       <c r="N953" s="5"/>
       <c r="O953" s="5"/>
@@ -36960,17 +36975,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="954" customHeight="1" ht="17.25">
       <c r="A954" s="1"/>
-      <c r="B954" s="10"/>
-      <c r="C954" s="10"/>
-      <c r="D954" s="11"/>
-      <c r="E954" s="11"/>
-      <c r="F954" s="10"/>
-      <c r="G954" s="11"/>
-      <c r="H954" s="11"/>
-      <c r="I954" s="11"/>
-      <c r="J954" s="11"/>
-      <c r="K954" s="11"/>
-      <c r="L954" s="11"/>
+      <c r="B954" s="11"/>
+      <c r="C954" s="11"/>
+      <c r="D954" s="12"/>
+      <c r="E954" s="12"/>
+      <c r="F954" s="11"/>
+      <c r="G954" s="12"/>
+      <c r="H954" s="12"/>
+      <c r="I954" s="12"/>
+      <c r="J954" s="12"/>
+      <c r="K954" s="12"/>
+      <c r="L954" s="12"/>
       <c r="M954" s="5"/>
       <c r="N954" s="5"/>
       <c r="O954" s="5"/>
@@ -36998,17 +37013,17 @@
     </row>
     <row x14ac:dyDescent="0.25" r="955" customHeight="1" ht="17.25">
       <c r="A955" s="1"/>
-      <c r="B955" s="10"/>
-      <c r="C955" s="10"/>
-      <c r="D955" s="11"/>
-      <c r="E955" s="11"/>
-      <c r="F955" s="10"/>
-      <c r="G955" s="11"/>
-      <c r="H955" s="11"/>
-      <c r="I955" s="11"/>
-      <c r="J955" s="11"/>
-      <c r="K955" s="11"/>
-      <c r="L955" s="11"/>
+      <c r="B955" s="11"/>
+      <c r="C955" s="11"/>
+      <c r="D955" s="12"/>
+      <c r="E955" s="12"/>
+      <c r="F955" s="11"/>
+      <c r="G955" s="12"/>
+      <c r="H955" s="12"/>
+      <c r="I955" s="12"/>
+      <c r="J955" s="12"/>
+      <c r="K955" s="12"/>
+      <c r="L955" s="12"/>
       <c r="M955" s="5"/>
       <c r="N955" s="5"/>
       <c r="O955" s="5"/>

</xml_diff>